<commit_message>
WALIA-05 Creatd patient entity
</commit_message>
<xml_diff>
--- a/walisClinic_design.xlsx
+++ b/walisClinic_design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t xml:space="preserve">Integer </t>
   </si>
@@ -129,9 +129,6 @@
     <t>Mehkar</t>
   </si>
   <si>
-    <t>History</t>
-  </si>
-  <si>
     <t>Dr Shelake</t>
   </si>
   <si>
@@ -139,13 +136,43 @@
   </si>
   <si>
     <t>Self</t>
+  </si>
+  <si>
+    <t>1:M</t>
+  </si>
+  <si>
+    <t>PatientId</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>bp</t>
+  </si>
+  <si>
+    <t>referBy</t>
+  </si>
+  <si>
+    <t>HistoryId</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Middlename</t>
+  </si>
+  <si>
+    <t>surname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +188,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -193,15 +228,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,6 +813,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -863,6 +912,9 @@
       <c r="J14" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="K14" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="L14" s="2" t="s">
         <v>20</v>
       </c>
@@ -958,91 +1010,129 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21" s="1"/>
+    </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="O22" t="s">
+      <c r="G22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="2">
+        <v>9063237318</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>67</v>
+      </c>
+      <c r="R23" s="2">
+        <v>164</v>
+      </c>
+      <c r="S23" s="2">
+        <v>56</v>
+      </c>
+      <c r="T23" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L23">
-        <v>9063237318</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="O24" s="2">
+        <v>2</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>63</v>
+      </c>
+      <c r="R24" s="2">
+        <v>165</v>
+      </c>
+      <c r="S24" s="2">
         <v>67</v>
       </c>
-      <c r="R23">
-        <v>164</v>
-      </c>
-      <c r="S23">
-        <v>56</v>
-      </c>
-      <c r="T23" t="s">
+      <c r="T24" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="O24">
-        <v>2</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>63</v>
-      </c>
-      <c r="R24">
-        <v>165</v>
-      </c>
-      <c r="S24">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="O25" s="2">
+        <v>3</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>45</v>
+      </c>
+      <c r="R25" s="2">
         <v>67</v>
       </c>
-      <c r="T24" t="s">
+      <c r="S25" s="2">
+        <v>78</v>
+      </c>
+      <c r="T25" s="2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="O25">
-        <v>3</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>45</v>
-      </c>
-      <c r="R25">
-        <v>67</v>
-      </c>
-      <c r="S25">
-        <v>78</v>
-      </c>
-      <c r="T25" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WALIA-06:Create User API implimented
</commit_message>
<xml_diff>
--- a/walisClinic_design.xlsx
+++ b/walisClinic_design.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sprint 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="design" sheetId="1" r:id="rId1"/>
+    <sheet name="sprint frist" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -802,7 +802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -1146,7 +1146,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
WALIA-07 Integrate thymeleaf with spring boot
</commit_message>
<xml_diff>
--- a/walisClinic_design.xlsx
+++ b/walisClinic_design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t xml:space="preserve">Integer </t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>surname</t>
+  </si>
+  <si>
+    <t>WALIA-07</t>
+  </si>
+  <si>
+    <t>Integrate Spring boot and Thymeleaf</t>
+  </si>
+  <si>
+    <t>Story_Id</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Owner</t>
   </si>
 </sst>
 </file>
@@ -1144,14 +1159,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="70.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>